<commit_message>
made the outpot anlysis
</commit_message>
<xml_diff>
--- a/dl_classification_notebook/csv_preformance/optuna_best_params.xlsx
+++ b/dl_classification_notebook/csv_preformance/optuna_best_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadav.k\Documents\DS\DL_classification\SAR_DL_classification\dl_classification_notebook\csv_preformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABF71DDE-8DC3-4A69-AC86-98DE425E0D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FDDE3C-6C3E-45C5-9EA9-B027D145ADEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63105" yWindow="3000" windowWidth="21600" windowHeight="11295" xr2:uid="{50B13CD7-B14F-4677-8170-C3912C80C9D5}"/>
+    <workbookView xWindow="63450" yWindow="3345" windowWidth="21600" windowHeight="11295" xr2:uid="{50B13CD7-B14F-4677-8170-C3912C80C9D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>